<commit_message>
use git_upload_now 2019/07/17 週三 15:08:17.14
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D01F5AD-C581-41E6-AD59-249C2E5CAC18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE82ECD7-2055-449D-B6D6-209D045E8C31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="3600" windowWidth="19725" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8835" yWindow="2160" windowWidth="14115" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>捷揚</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,15 +59,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0905 300 313</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>新光</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>中興</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有無監視器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保險內容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>竊盜險40萬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0982 819 655林先生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>繳一年算13個月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用網路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固定基地台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配合鎖匠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可否假日安裝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安裝前幾天聯絡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高理賠200倍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>當天聯絡就可以</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以星期日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0905 300 313許先生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以星期日(要安排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三天之前(要發包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固定基地台，可支援sim卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>835 7811</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -394,69 +466,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+      <c r="D3">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use git_upload_now 2019/07/17 週三 15:11:38.56
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE82ECD7-2055-449D-B6D6-209D045E8C31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1A8F54-3817-4AEE-9BEE-4C34853635B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="2160" windowWidth="14115" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10875" yWindow="2100" windowWidth="14115" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>捷揚</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,10 +92,6 @@
   </si>
   <si>
     <t>使用網路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>固定基地台</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -469,7 +465,7 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -554,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -562,15 +558,15 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -581,24 +577,24 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -606,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -614,7 +610,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use git_upload_now 2019/07/18 週四 11:42:56.80
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1A8F54-3817-4AEE-9BEE-4C34853635B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1769BB-F8F2-4E53-B65D-8D61DDFB94F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10875" yWindow="2100" windowWidth="14115" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="2190" windowWidth="14115" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>捷揚</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,7 +135,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>835 7811</t>
+    <t>訂金多少</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施工時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安裝需要的證明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防盜器有線無線</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1600~2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0953 905 536蕭先生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以刷卡嗎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>印章(契約要圖面 要畫個圖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3~4小時不包含窗戶?????</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鐵捲門那些都是無線的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以刷卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21160含稅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1600未稅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000免稅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紅外線裝置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放三四隻紅外線</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -143,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +215,29 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -179,9 +262,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -462,156 +547,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1">
         <v>2000</v>
       </c>
-      <c r="D3">
-        <v>1600</v>
-      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>1000</v>
-      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
use git_upload_now 2019/07/22 週一 12:07:29.48
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1769BB-F8F2-4E53-B65D-8D61DDFB94F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D002141-CB3A-45DF-9A76-8E47C6A2BFFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="2190" windowWidth="14115" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>捷揚</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,6 +196,26 @@
   </si>
   <si>
     <t>放三四隻紅外線</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天威</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200 / 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>繳11個月算12個月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無監視器 / 有4隻監視器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿秋 0933 185 241</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -547,264 +567,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E24"/>
+  <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="3" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="1"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>3000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="3"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
use git_upload_now 2019/07/22 週一 15:54:54.05
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D002141-CB3A-45DF-9A76-8E47C6A2BFFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7123138-6494-45FD-940F-3B186F211FF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>捷揚</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -215,7 +215,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>阿秋 0933 185 241</t>
+    <t>固定基地台(可支援sim卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男的 洪啟煌 0933 185 241</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註: 很愛聊天…電話費QQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有線無線都可以</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200*11 / 1500*11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>就先聯絡畫圖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有認識的 但可能沒比較便宜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,7 +602,7 @@
   <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -662,7 +694,9 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>4</v>
@@ -705,7 +739,9 @@
       <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>26</v>
@@ -718,7 +754,9 @@
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>11</v>
@@ -744,7 +782,9 @@
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>25</v>
@@ -757,7 +797,9 @@
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
@@ -768,7 +810,9 @@
       <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
@@ -779,7 +823,9 @@
       <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
@@ -790,7 +836,9 @@
       <c r="C16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
@@ -801,7 +849,9 @@
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
@@ -812,7 +862,9 @@
       <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
@@ -824,7 +876,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>32</v>
@@ -836,7 +888,9 @@
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>

</xml_diff>

<commit_message>
use git_upload_now 2019/07/22 週一 16:27:07.55
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7123138-6494-45FD-940F-3B186F211FF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A28387-F99D-4723-A6DA-38E331AF6BCB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,10 +227,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>男的 洪啟煌 0933 185 241</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>備註: 很愛聊天…電話費QQ</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -239,15 +235,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1200*11 / 1500*11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>就先聯絡畫圖</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>有認識的 但可能沒比較便宜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男的 洪志煌 0933 185 241</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200*11 / 1500*11 (要再加稅)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -602,7 +602,7 @@
   <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -755,7 +755,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
@@ -783,7 +783,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
@@ -798,7 +798,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -863,7 +863,7 @@
         <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -876,7 +876,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>32</v>
@@ -889,7 +889,7 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>

</xml_diff>

<commit_message>
use git_upload_now 2019/07/29 週一 20:41:35.77
</commit_message>
<xml_diff>
--- a/281/保全.xlsx
+++ b/281/保全.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U\git\ud8\281\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A28387-F99D-4723-A6DA-38E331AF6BCB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA92CCD-23BD-4C02-ACBE-DA923084C19B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,11 +243,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>男的 洪志煌 0933 185 241</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1200*11 / 1500*11 (要再加稅)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洪啟煌 0933 185 241</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -602,7 +602,7 @@
   <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -876,7 +876,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>32</v>

</xml_diff>